<commit_message>
75'e kadar bölüm eklendi - en
</commit_message>
<xml_diff>
--- a/Levels/en/Wordlist.xlsx
+++ b/Levels/en/Wordlist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="775">
   <si>
     <t>id</t>
   </si>
@@ -1927,18 +1927,443 @@
   </si>
   <si>
     <t>RANG</t>
+  </si>
+  <si>
+    <t>D,N,H,A,Y</t>
+  </si>
+  <si>
+    <t>HAND</t>
+  </si>
+  <si>
+    <t>HAD</t>
+  </si>
+  <si>
+    <t>HAY</t>
+  </si>
+  <si>
+    <t>HANDY</t>
+  </si>
+  <si>
+    <t>O,R,U,S,Y</t>
+  </si>
+  <si>
+    <t>YOURS</t>
+  </si>
+  <si>
+    <t>SOUR</t>
+  </si>
+  <si>
+    <t>YOUR</t>
+  </si>
+  <si>
+    <t>SOY</t>
+  </si>
+  <si>
+    <t>YOU</t>
+  </si>
+  <si>
+    <t>I,D,A,R,O</t>
+  </si>
+  <si>
+    <t>ROAD</t>
+  </si>
+  <si>
+    <t>RAID</t>
+  </si>
+  <si>
+    <t>ROD</t>
+  </si>
+  <si>
+    <t>RADIO</t>
+  </si>
+  <si>
+    <t>AIR</t>
+  </si>
+  <si>
+    <t>T,S,U,N,R</t>
+  </si>
+  <si>
+    <t>RUST</t>
+  </si>
+  <si>
+    <t>NUT</t>
+  </si>
+  <si>
+    <t>RUNS</t>
+  </si>
+  <si>
+    <t>STUN</t>
+  </si>
+  <si>
+    <t>SUN</t>
+  </si>
+  <si>
+    <t>TURNS</t>
+  </si>
+  <si>
+    <t>RUN</t>
+  </si>
+  <si>
+    <t>TURN</t>
+  </si>
+  <si>
+    <t>T,S,H,S,O</t>
+  </si>
+  <si>
+    <t>SHOT</t>
+  </si>
+  <si>
+    <t>HOST</t>
+  </si>
+  <si>
+    <t>SHOTS</t>
+  </si>
+  <si>
+    <t>HOSTS</t>
+  </si>
+  <si>
+    <t>TOSS</t>
+  </si>
+  <si>
+    <t>E,N,D,Y,E</t>
+  </si>
+  <si>
+    <t>DYE</t>
+  </si>
+  <si>
+    <t>NEED</t>
+  </si>
+  <si>
+    <t>NEEDY</t>
+  </si>
+  <si>
+    <t>DENY</t>
+  </si>
+  <si>
+    <t>P,W,N,R,A</t>
+  </si>
+  <si>
+    <t>NAP</t>
+  </si>
+  <si>
+    <t>PRAWN</t>
+  </si>
+  <si>
+    <t>WARN</t>
+  </si>
+  <si>
+    <t>PAWN</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>L,E,W,O,H</t>
+  </si>
+  <si>
+    <t>HOW</t>
+  </si>
+  <si>
+    <t>HOWL</t>
+  </si>
+  <si>
+    <t>WHOLE</t>
+  </si>
+  <si>
+    <t>WHO</t>
+  </si>
+  <si>
+    <t>HOLE</t>
+  </si>
+  <si>
+    <t>N,P,C,I,H</t>
+  </si>
+  <si>
+    <t>CHIN</t>
+  </si>
+  <si>
+    <t>CHIP</t>
+  </si>
+  <si>
+    <t>INCH</t>
+  </si>
+  <si>
+    <t>PINCH</t>
+  </si>
+  <si>
+    <t>M,A,E,T,N</t>
+  </si>
+  <si>
+    <t>NEAT</t>
+  </si>
+  <si>
+    <t>MANE</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>MEANT</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>TAME</t>
+  </si>
+  <si>
+    <t>B,C,A,H,E</t>
+  </si>
+  <si>
+    <t>CAB</t>
+  </si>
+  <si>
+    <t>ACE</t>
+  </si>
+  <si>
+    <t>ACHE</t>
+  </si>
+  <si>
+    <t>EACH</t>
+  </si>
+  <si>
+    <t>BEACH</t>
+  </si>
+  <si>
+    <t>A,Y,S,L,T</t>
+  </si>
+  <si>
+    <t>LAYS</t>
+  </si>
+  <si>
+    <t>SALTY</t>
+  </si>
+  <si>
+    <t>STAY</t>
+  </si>
+  <si>
+    <t>A,E,R,F,M</t>
+  </si>
+  <si>
+    <t>FAR</t>
+  </si>
+  <si>
+    <t>ARM</t>
+  </si>
+  <si>
+    <t>FRAME</t>
+  </si>
+  <si>
+    <t>FARE</t>
+  </si>
+  <si>
+    <t>FARM</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>FEAR</t>
+  </si>
+  <si>
+    <t>FAME</t>
+  </si>
+  <si>
+    <t>MARE</t>
+  </si>
+  <si>
+    <t>K,O,C,A,L</t>
+  </si>
+  <si>
+    <t>OAK</t>
+  </si>
+  <si>
+    <t>COLA</t>
+  </si>
+  <si>
+    <t>CLOAK</t>
+  </si>
+  <si>
+    <t>LOCK</t>
+  </si>
+  <si>
+    <t>COAL</t>
+  </si>
+  <si>
+    <t>LACK</t>
+  </si>
+  <si>
+    <t>W,O,R,S,T</t>
+  </si>
+  <si>
+    <t>TWO</t>
+  </si>
+  <si>
+    <t>ROW</t>
+  </si>
+  <si>
+    <t>SORT</t>
+  </si>
+  <si>
+    <t>ROT</t>
+  </si>
+  <si>
+    <t>ROWS</t>
+  </si>
+  <si>
+    <t>WORST</t>
+  </si>
+  <si>
+    <t>SOW</t>
+  </si>
+  <si>
+    <t>O,L,S,T,O</t>
+  </si>
+  <si>
+    <t>SOLO</t>
+  </si>
+  <si>
+    <t>TOOLS</t>
+  </si>
+  <si>
+    <t>SLOT</t>
+  </si>
+  <si>
+    <t>LOTS</t>
+  </si>
+  <si>
+    <t>TOOL</t>
+  </si>
+  <si>
+    <t>LOST</t>
+  </si>
+  <si>
+    <t>LOOT</t>
+  </si>
+  <si>
+    <t>STOOL</t>
+  </si>
+  <si>
+    <t>I,G,D,N,R</t>
+  </si>
+  <si>
+    <t>GRID</t>
+  </si>
+  <si>
+    <t>DIG</t>
+  </si>
+  <si>
+    <t>GRIND</t>
+  </si>
+  <si>
+    <t>C,A,M,L,P</t>
+  </si>
+  <si>
+    <t>CAM</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>MAP</t>
+  </si>
+  <si>
+    <t>CAMP</t>
+  </si>
+  <si>
+    <t>CLAMP</t>
+  </si>
+  <si>
+    <t>LAMP</t>
+  </si>
+  <si>
+    <t>PALM</t>
+  </si>
+  <si>
+    <t>CLAP</t>
+  </si>
+  <si>
+    <t>A,B,T,H,I</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>BATH</t>
+  </si>
+  <si>
+    <t>TAB</t>
+  </si>
+  <si>
+    <t>BIT</t>
+  </si>
+  <si>
+    <t>HABIT</t>
+  </si>
+  <si>
+    <t>BAIT</t>
+  </si>
+  <si>
+    <t>E,L,R,T,A</t>
+  </si>
+  <si>
+    <t>ALTER</t>
+  </si>
+  <si>
+    <t>TEAR</t>
+  </si>
+  <si>
+    <t>REAL</t>
+  </si>
+  <si>
+    <t>EARL</t>
+  </si>
+  <si>
+    <t>RATE</t>
+  </si>
+  <si>
+    <t>ALERT</t>
+  </si>
+  <si>
+    <t>LATER</t>
+  </si>
+  <si>
+    <t>A,C,H,S,R</t>
+  </si>
+  <si>
+    <t>SCAR</t>
+  </si>
+  <si>
+    <t>CRASH</t>
+  </si>
+  <si>
+    <t>ARCH</t>
+  </si>
+  <si>
+    <t>RASH</t>
+  </si>
+  <si>
+    <t>CARS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1994,18 +2419,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2286,10 +2713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E359"/>
+  <dimension ref="A1:F526"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A346" workbookViewId="0">
-      <selection activeCell="E360" sqref="E360"/>
+    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
+      <selection activeCell="F360" sqref="F360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8036,7 +8463,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>54</v>
       </c>
@@ -8050,7 +8477,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>54</v>
       </c>
@@ -8064,7 +8491,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>54</v>
       </c>
@@ -8078,7 +8505,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>54</v>
       </c>
@@ -8092,7 +8519,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>54</v>
       </c>
@@ -8106,7 +8533,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>54</v>
       </c>
@@ -8120,7 +8547,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>54</v>
       </c>
@@ -8131,6 +8558,2345 @@
         <v>45</v>
       </c>
       <c r="E359" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>55</v>
+      </c>
+      <c r="B360" t="s">
+        <v>636</v>
+      </c>
+      <c r="C360" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="E360" t="s">
+        <v>116</v>
+      </c>
+      <c r="F360" s="8"/>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>55</v>
+      </c>
+      <c r="B361" t="s">
+        <v>636</v>
+      </c>
+      <c r="C361" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="E361" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>55</v>
+      </c>
+      <c r="B362" t="s">
+        <v>636</v>
+      </c>
+      <c r="C362" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="E362" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>55</v>
+      </c>
+      <c r="B363" t="s">
+        <v>636</v>
+      </c>
+      <c r="C363" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E363" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>55</v>
+      </c>
+      <c r="B364" t="s">
+        <v>636</v>
+      </c>
+      <c r="C364" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="E364" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>55</v>
+      </c>
+      <c r="B365" t="s">
+        <v>636</v>
+      </c>
+      <c r="C365" s="7" t="s">
+        <v>640</v>
+      </c>
+      <c r="E365" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>55</v>
+      </c>
+      <c r="B366" t="s">
+        <v>636</v>
+      </c>
+      <c r="C366" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="E366" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>56</v>
+      </c>
+      <c r="B367" t="s">
+        <v>641</v>
+      </c>
+      <c r="C367" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="E367" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>56</v>
+      </c>
+      <c r="B368" t="s">
+        <v>641</v>
+      </c>
+      <c r="C368" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="E368" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>56</v>
+      </c>
+      <c r="B369" t="s">
+        <v>641</v>
+      </c>
+      <c r="C369" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="E369" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>56</v>
+      </c>
+      <c r="B370" t="s">
+        <v>641</v>
+      </c>
+      <c r="C370" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E370" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>56</v>
+      </c>
+      <c r="B371" t="s">
+        <v>641</v>
+      </c>
+      <c r="C371" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="E371" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>56</v>
+      </c>
+      <c r="B372" t="s">
+        <v>641</v>
+      </c>
+      <c r="C372" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="E372" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>57</v>
+      </c>
+      <c r="B373" t="s">
+        <v>647</v>
+      </c>
+      <c r="C373" s="7" t="s">
+        <v>648</v>
+      </c>
+      <c r="E373" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>57</v>
+      </c>
+      <c r="B374" t="s">
+        <v>647</v>
+      </c>
+      <c r="C374" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E374" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>57</v>
+      </c>
+      <c r="B375" t="s">
+        <v>647</v>
+      </c>
+      <c r="C375" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="E375" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>57</v>
+      </c>
+      <c r="B376" t="s">
+        <v>647</v>
+      </c>
+      <c r="C376" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="E376" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>57</v>
+      </c>
+      <c r="B377" t="s">
+        <v>647</v>
+      </c>
+      <c r="C377" s="7" t="s">
+        <v>651</v>
+      </c>
+      <c r="E377" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>57</v>
+      </c>
+      <c r="B378" t="s">
+        <v>647</v>
+      </c>
+      <c r="C378" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="E378" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>58</v>
+      </c>
+      <c r="B379" t="s">
+        <v>653</v>
+      </c>
+      <c r="C379" s="7" t="s">
+        <v>654</v>
+      </c>
+      <c r="E379" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>58</v>
+      </c>
+      <c r="B380" t="s">
+        <v>653</v>
+      </c>
+      <c r="C380" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="E380" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>58</v>
+      </c>
+      <c r="B381" t="s">
+        <v>653</v>
+      </c>
+      <c r="C381" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="E381" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>58</v>
+      </c>
+      <c r="B382" t="s">
+        <v>653</v>
+      </c>
+      <c r="C382" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="E382" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>58</v>
+      </c>
+      <c r="B383" t="s">
+        <v>653</v>
+      </c>
+      <c r="C383" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="E383" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>58</v>
+      </c>
+      <c r="B384" t="s">
+        <v>653</v>
+      </c>
+      <c r="C384" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="E384" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>58</v>
+      </c>
+      <c r="B385" t="s">
+        <v>653</v>
+      </c>
+      <c r="C385" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="E385" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>58</v>
+      </c>
+      <c r="B386" t="s">
+        <v>653</v>
+      </c>
+      <c r="C386" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="E386" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>59</v>
+      </c>
+      <c r="B387" t="s">
+        <v>662</v>
+      </c>
+      <c r="C387" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E387" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>59</v>
+      </c>
+      <c r="B388" t="s">
+        <v>662</v>
+      </c>
+      <c r="C388" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="E388" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>59</v>
+      </c>
+      <c r="B389" t="s">
+        <v>662</v>
+      </c>
+      <c r="C389" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="E389" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>59</v>
+      </c>
+      <c r="B390" t="s">
+        <v>662</v>
+      </c>
+      <c r="C390" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="E390" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>59</v>
+      </c>
+      <c r="B391" t="s">
+        <v>662</v>
+      </c>
+      <c r="C391" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="E391" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>59</v>
+      </c>
+      <c r="B392" t="s">
+        <v>662</v>
+      </c>
+      <c r="C392" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="E392" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>60</v>
+      </c>
+      <c r="B393" t="s">
+        <v>668</v>
+      </c>
+      <c r="C393" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E393" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>60</v>
+      </c>
+      <c r="B394" t="s">
+        <v>668</v>
+      </c>
+      <c r="C394" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E394" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>60</v>
+      </c>
+      <c r="B395" t="s">
+        <v>668</v>
+      </c>
+      <c r="C395" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="E395" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>60</v>
+      </c>
+      <c r="B396" t="s">
+        <v>668</v>
+      </c>
+      <c r="C396" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="E396" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>60</v>
+      </c>
+      <c r="B397" t="s">
+        <v>668</v>
+      </c>
+      <c r="C397" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="E397" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>60</v>
+      </c>
+      <c r="B398" t="s">
+        <v>668</v>
+      </c>
+      <c r="C398" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E398" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>60</v>
+      </c>
+      <c r="B399" t="s">
+        <v>668</v>
+      </c>
+      <c r="C399" s="7" t="s">
+        <v>672</v>
+      </c>
+      <c r="E399" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>61</v>
+      </c>
+      <c r="B400" t="s">
+        <v>673</v>
+      </c>
+      <c r="C400" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="E400" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>61</v>
+      </c>
+      <c r="B401" t="s">
+        <v>673</v>
+      </c>
+      <c r="C401" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="E401" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>61</v>
+      </c>
+      <c r="B402" t="s">
+        <v>673</v>
+      </c>
+      <c r="C402" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="E402" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>61</v>
+      </c>
+      <c r="B403" t="s">
+        <v>673</v>
+      </c>
+      <c r="C403" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="E403" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>61</v>
+      </c>
+      <c r="B404" t="s">
+        <v>673</v>
+      </c>
+      <c r="C404" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="E404" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>61</v>
+      </c>
+      <c r="B405" t="s">
+        <v>673</v>
+      </c>
+      <c r="C405" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="E405" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>61</v>
+      </c>
+      <c r="B406" t="s">
+        <v>673</v>
+      </c>
+      <c r="C406" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="E406" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>61</v>
+      </c>
+      <c r="B407" t="s">
+        <v>673</v>
+      </c>
+      <c r="C407" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="E407" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>61</v>
+      </c>
+      <c r="B408" t="s">
+        <v>673</v>
+      </c>
+      <c r="C408" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="E408" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>61</v>
+      </c>
+      <c r="B409" t="s">
+        <v>673</v>
+      </c>
+      <c r="C409" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="E409" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>62</v>
+      </c>
+      <c r="B410" t="s">
+        <v>679</v>
+      </c>
+      <c r="C410" s="7" t="s">
+        <v>680</v>
+      </c>
+      <c r="E410" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>62</v>
+      </c>
+      <c r="B411" t="s">
+        <v>679</v>
+      </c>
+      <c r="C411" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="E411" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>62</v>
+      </c>
+      <c r="B412" t="s">
+        <v>679</v>
+      </c>
+      <c r="C412" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="E412" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>62</v>
+      </c>
+      <c r="B413" t="s">
+        <v>679</v>
+      </c>
+      <c r="C413" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="E413" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>62</v>
+      </c>
+      <c r="B414" t="s">
+        <v>679</v>
+      </c>
+      <c r="C414" s="7" t="s">
+        <v>682</v>
+      </c>
+      <c r="E414" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>62</v>
+      </c>
+      <c r="B415" t="s">
+        <v>679</v>
+      </c>
+      <c r="C415" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="E415" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>62</v>
+      </c>
+      <c r="B416" t="s">
+        <v>679</v>
+      </c>
+      <c r="C416" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="E416" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>63</v>
+      </c>
+      <c r="B417" t="s">
+        <v>685</v>
+      </c>
+      <c r="C417" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="E417" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>63</v>
+      </c>
+      <c r="B418" t="s">
+        <v>685</v>
+      </c>
+      <c r="C418" s="7" t="s">
+        <v>686</v>
+      </c>
+      <c r="E418" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>63</v>
+      </c>
+      <c r="B419" t="s">
+        <v>685</v>
+      </c>
+      <c r="C419" s="7" t="s">
+        <v>687</v>
+      </c>
+      <c r="E419" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>63</v>
+      </c>
+      <c r="B420" t="s">
+        <v>685</v>
+      </c>
+      <c r="C420" s="7" t="s">
+        <v>688</v>
+      </c>
+      <c r="E420" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>63</v>
+      </c>
+      <c r="B421" t="s">
+        <v>685</v>
+      </c>
+      <c r="C421" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="E421" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>63</v>
+      </c>
+      <c r="B422" t="s">
+        <v>685</v>
+      </c>
+      <c r="C422" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="E422" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>64</v>
+      </c>
+      <c r="B423" t="s">
+        <v>690</v>
+      </c>
+      <c r="C423" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E423" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A424">
+        <v>64</v>
+      </c>
+      <c r="B424" t="s">
+        <v>690</v>
+      </c>
+      <c r="C424" s="7" t="s">
+        <v>691</v>
+      </c>
+      <c r="E424" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>64</v>
+      </c>
+      <c r="B425" t="s">
+        <v>690</v>
+      </c>
+      <c r="C425" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="E425" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>64</v>
+      </c>
+      <c r="B426" t="s">
+        <v>690</v>
+      </c>
+      <c r="C426" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="E426" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A427">
+        <v>64</v>
+      </c>
+      <c r="B427" t="s">
+        <v>690</v>
+      </c>
+      <c r="C427" s="7" t="s">
+        <v>694</v>
+      </c>
+      <c r="E427" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A428">
+        <v>64</v>
+      </c>
+      <c r="B428" t="s">
+        <v>690</v>
+      </c>
+      <c r="C428" s="7" t="s">
+        <v>695</v>
+      </c>
+      <c r="E428" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A429">
+        <v>64</v>
+      </c>
+      <c r="B429" t="s">
+        <v>690</v>
+      </c>
+      <c r="C429" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E429" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>64</v>
+      </c>
+      <c r="B430" t="s">
+        <v>690</v>
+      </c>
+      <c r="C430" s="7" t="s">
+        <v>696</v>
+      </c>
+      <c r="E430" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>64</v>
+      </c>
+      <c r="B431" t="s">
+        <v>690</v>
+      </c>
+      <c r="C431" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E431" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A432">
+        <v>65</v>
+      </c>
+      <c r="B432" t="s">
+        <v>697</v>
+      </c>
+      <c r="C432" s="7" t="s">
+        <v>698</v>
+      </c>
+      <c r="E432" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>65</v>
+      </c>
+      <c r="B433" t="s">
+        <v>697</v>
+      </c>
+      <c r="C433" s="7" t="s">
+        <v>699</v>
+      </c>
+      <c r="E433" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A434">
+        <v>65</v>
+      </c>
+      <c r="B434" t="s">
+        <v>697</v>
+      </c>
+      <c r="C434" s="7" t="s">
+        <v>700</v>
+      </c>
+      <c r="E434" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A435">
+        <v>65</v>
+      </c>
+      <c r="B435" t="s">
+        <v>697</v>
+      </c>
+      <c r="C435" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="E435" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A436">
+        <v>65</v>
+      </c>
+      <c r="B436" t="s">
+        <v>697</v>
+      </c>
+      <c r="C436" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="E436" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A437">
+        <v>66</v>
+      </c>
+      <c r="B437" t="s">
+        <v>703</v>
+      </c>
+      <c r="C437" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E437" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A438">
+        <v>66</v>
+      </c>
+      <c r="B438" t="s">
+        <v>703</v>
+      </c>
+      <c r="C438" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="E438" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A439">
+        <v>66</v>
+      </c>
+      <c r="B439" t="s">
+        <v>703</v>
+      </c>
+      <c r="C439" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E439" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A440">
+        <v>66</v>
+      </c>
+      <c r="B440" t="s">
+        <v>703</v>
+      </c>
+      <c r="C440" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="E440" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A441">
+        <v>66</v>
+      </c>
+      <c r="B441" t="s">
+        <v>703</v>
+      </c>
+      <c r="C441" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="E441" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A442">
+        <v>66</v>
+      </c>
+      <c r="B442" t="s">
+        <v>703</v>
+      </c>
+      <c r="C442" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="E442" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A443">
+        <v>66</v>
+      </c>
+      <c r="B443" t="s">
+        <v>703</v>
+      </c>
+      <c r="C443" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E443" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A444">
+        <v>66</v>
+      </c>
+      <c r="B444" t="s">
+        <v>703</v>
+      </c>
+      <c r="C444" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="E444" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A445">
+        <v>67</v>
+      </c>
+      <c r="B445" t="s">
+        <v>707</v>
+      </c>
+      <c r="C445" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="E445" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A446">
+        <v>67</v>
+      </c>
+      <c r="B446" t="s">
+        <v>707</v>
+      </c>
+      <c r="C446" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="E446" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A447">
+        <v>67</v>
+      </c>
+      <c r="B447" t="s">
+        <v>707</v>
+      </c>
+      <c r="C447" s="7" t="s">
+        <v>710</v>
+      </c>
+      <c r="E447" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A448">
+        <v>67</v>
+      </c>
+      <c r="B448" t="s">
+        <v>707</v>
+      </c>
+      <c r="C448" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E448" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>67</v>
+      </c>
+      <c r="B449" t="s">
+        <v>707</v>
+      </c>
+      <c r="C449" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="E449" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>67</v>
+      </c>
+      <c r="B450" t="s">
+        <v>707</v>
+      </c>
+      <c r="C450" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="E450" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A451">
+        <v>67</v>
+      </c>
+      <c r="B451" t="s">
+        <v>707</v>
+      </c>
+      <c r="C451" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="E451" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A452">
+        <v>67</v>
+      </c>
+      <c r="B452" t="s">
+        <v>707</v>
+      </c>
+      <c r="C452" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="E452" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A453">
+        <v>67</v>
+      </c>
+      <c r="B453" t="s">
+        <v>707</v>
+      </c>
+      <c r="C453" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="E453" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A454">
+        <v>67</v>
+      </c>
+      <c r="B454" t="s">
+        <v>707</v>
+      </c>
+      <c r="C454" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E454" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A455">
+        <v>67</v>
+      </c>
+      <c r="B455" t="s">
+        <v>707</v>
+      </c>
+      <c r="C455" s="7" t="s">
+        <v>716</v>
+      </c>
+      <c r="E455" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>68</v>
+      </c>
+      <c r="B456" t="s">
+        <v>717</v>
+      </c>
+      <c r="C456" s="7" t="s">
+        <v>718</v>
+      </c>
+      <c r="E456" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A457">
+        <v>68</v>
+      </c>
+      <c r="B457" t="s">
+        <v>717</v>
+      </c>
+      <c r="C457" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="E457" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A458">
+        <v>68</v>
+      </c>
+      <c r="B458" t="s">
+        <v>717</v>
+      </c>
+      <c r="C458" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="E458" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A459">
+        <v>68</v>
+      </c>
+      <c r="B459" t="s">
+        <v>717</v>
+      </c>
+      <c r="C459" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="E459" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A460">
+        <v>68</v>
+      </c>
+      <c r="B460" t="s">
+        <v>717</v>
+      </c>
+      <c r="C460" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="E460" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A461">
+        <v>68</v>
+      </c>
+      <c r="B461" t="s">
+        <v>717</v>
+      </c>
+      <c r="C461" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="E461" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A462">
+        <v>69</v>
+      </c>
+      <c r="B462" t="s">
+        <v>724</v>
+      </c>
+      <c r="C462" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="E462" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A463">
+        <v>69</v>
+      </c>
+      <c r="B463" t="s">
+        <v>724</v>
+      </c>
+      <c r="C463" s="7" t="s">
+        <v>726</v>
+      </c>
+      <c r="E463" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A464">
+        <v>69</v>
+      </c>
+      <c r="B464" t="s">
+        <v>724</v>
+      </c>
+      <c r="C464" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="E464" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A465">
+        <v>69</v>
+      </c>
+      <c r="B465" t="s">
+        <v>724</v>
+      </c>
+      <c r="C465" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E465" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A466">
+        <v>69</v>
+      </c>
+      <c r="B466" t="s">
+        <v>724</v>
+      </c>
+      <c r="C466" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="E466" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A467">
+        <v>69</v>
+      </c>
+      <c r="B467" t="s">
+        <v>724</v>
+      </c>
+      <c r="C467" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="E467" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A468">
+        <v>69</v>
+      </c>
+      <c r="B468" t="s">
+        <v>724</v>
+      </c>
+      <c r="C468" s="7" t="s">
+        <v>731</v>
+      </c>
+      <c r="E468" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A469">
+        <v>70</v>
+      </c>
+      <c r="B469" t="s">
+        <v>732</v>
+      </c>
+      <c r="C469" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="E469" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A470">
+        <v>70</v>
+      </c>
+      <c r="B470" t="s">
+        <v>732</v>
+      </c>
+      <c r="C470" s="7" t="s">
+        <v>734</v>
+      </c>
+      <c r="E470" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A471">
+        <v>70</v>
+      </c>
+      <c r="B471" t="s">
+        <v>732</v>
+      </c>
+      <c r="C471" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="E471" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A472">
+        <v>70</v>
+      </c>
+      <c r="B472" t="s">
+        <v>732</v>
+      </c>
+      <c r="C472" s="7" t="s">
+        <v>736</v>
+      </c>
+      <c r="E472" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A473">
+        <v>70</v>
+      </c>
+      <c r="B473" t="s">
+        <v>732</v>
+      </c>
+      <c r="C473" s="7" t="s">
+        <v>737</v>
+      </c>
+      <c r="E473" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A474">
+        <v>70</v>
+      </c>
+      <c r="B474" t="s">
+        <v>732</v>
+      </c>
+      <c r="C474" s="7" t="s">
+        <v>738</v>
+      </c>
+      <c r="E474" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A475">
+        <v>70</v>
+      </c>
+      <c r="B475" t="s">
+        <v>732</v>
+      </c>
+      <c r="C475" s="7" t="s">
+        <v>739</v>
+      </c>
+      <c r="E475" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A476">
+        <v>70</v>
+      </c>
+      <c r="B476" t="s">
+        <v>732</v>
+      </c>
+      <c r="C476" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="E476" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="477" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A477">
+        <v>70</v>
+      </c>
+      <c r="B477" t="s">
+        <v>732</v>
+      </c>
+      <c r="C477" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="E477" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A478">
+        <v>71</v>
+      </c>
+      <c r="B478" t="s">
+        <v>741</v>
+      </c>
+      <c r="C478" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E478" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A479">
+        <v>71</v>
+      </c>
+      <c r="B479" t="s">
+        <v>741</v>
+      </c>
+      <c r="C479" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="E479" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A480">
+        <v>71</v>
+      </c>
+      <c r="B480" t="s">
+        <v>741</v>
+      </c>
+      <c r="C480" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="E480" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A481">
+        <v>71</v>
+      </c>
+      <c r="B481" t="s">
+        <v>741</v>
+      </c>
+      <c r="C481" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E481" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A482">
+        <v>71</v>
+      </c>
+      <c r="B482" t="s">
+        <v>741</v>
+      </c>
+      <c r="C482" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="E482" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A483">
+        <v>71</v>
+      </c>
+      <c r="B483" t="s">
+        <v>741</v>
+      </c>
+      <c r="C483" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="E483" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A484">
+        <v>71</v>
+      </c>
+      <c r="B484" t="s">
+        <v>741</v>
+      </c>
+      <c r="C484" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E484" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A485">
+        <v>71</v>
+      </c>
+      <c r="B485" t="s">
+        <v>741</v>
+      </c>
+      <c r="C485" s="7" t="s">
+        <v>744</v>
+      </c>
+      <c r="E485" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A486">
+        <v>72</v>
+      </c>
+      <c r="B486" t="s">
+        <v>745</v>
+      </c>
+      <c r="C486" s="7" t="s">
+        <v>746</v>
+      </c>
+      <c r="E486" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A487">
+        <v>72</v>
+      </c>
+      <c r="B487" t="s">
+        <v>745</v>
+      </c>
+      <c r="C487" s="7" t="s">
+        <v>747</v>
+      </c>
+      <c r="E487" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A488">
+        <v>72</v>
+      </c>
+      <c r="B488" t="s">
+        <v>745</v>
+      </c>
+      <c r="C488" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="E488" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A489">
+        <v>72</v>
+      </c>
+      <c r="B489" t="s">
+        <v>745</v>
+      </c>
+      <c r="C489" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="E489" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A490">
+        <v>72</v>
+      </c>
+      <c r="B490" t="s">
+        <v>745</v>
+      </c>
+      <c r="C490" s="7" t="s">
+        <v>750</v>
+      </c>
+      <c r="E490" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A491">
+        <v>72</v>
+      </c>
+      <c r="B491" t="s">
+        <v>745</v>
+      </c>
+      <c r="C491" s="7" t="s">
+        <v>751</v>
+      </c>
+      <c r="E491" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A492">
+        <v>72</v>
+      </c>
+      <c r="B492" t="s">
+        <v>745</v>
+      </c>
+      <c r="C492" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E492" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A493">
+        <v>72</v>
+      </c>
+      <c r="B493" t="s">
+        <v>745</v>
+      </c>
+      <c r="C493" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E493" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="494" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A494">
+        <v>72</v>
+      </c>
+      <c r="B494" t="s">
+        <v>745</v>
+      </c>
+      <c r="C494" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E494" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="495" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A495">
+        <v>72</v>
+      </c>
+      <c r="B495" t="s">
+        <v>745</v>
+      </c>
+      <c r="C495" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E495" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="496" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A496">
+        <v>72</v>
+      </c>
+      <c r="B496" t="s">
+        <v>745</v>
+      </c>
+      <c r="C496" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="E496" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="497" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A497">
+        <v>72</v>
+      </c>
+      <c r="B497" t="s">
+        <v>745</v>
+      </c>
+      <c r="C497" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="E497" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="498" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A498">
+        <v>73</v>
+      </c>
+      <c r="B498" t="s">
+        <v>754</v>
+      </c>
+      <c r="C498" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E498" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="499" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A499">
+        <v>73</v>
+      </c>
+      <c r="B499" t="s">
+        <v>754</v>
+      </c>
+      <c r="C499" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="E499" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="500" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A500">
+        <v>73</v>
+      </c>
+      <c r="B500" t="s">
+        <v>754</v>
+      </c>
+      <c r="C500" s="7" t="s">
+        <v>756</v>
+      </c>
+      <c r="E500" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="501" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A501">
+        <v>73</v>
+      </c>
+      <c r="B501" t="s">
+        <v>754</v>
+      </c>
+      <c r="C501" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="E501" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="502" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A502">
+        <v>73</v>
+      </c>
+      <c r="B502" t="s">
+        <v>754</v>
+      </c>
+      <c r="C502" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="E502" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="503" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A503">
+        <v>73</v>
+      </c>
+      <c r="B503" t="s">
+        <v>754</v>
+      </c>
+      <c r="C503" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="E503" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="504" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A504">
+        <v>73</v>
+      </c>
+      <c r="B504" t="s">
+        <v>754</v>
+      </c>
+      <c r="C504" s="7" t="s">
+        <v>760</v>
+      </c>
+      <c r="E504" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="505" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A505">
+        <v>73</v>
+      </c>
+      <c r="B505" t="s">
+        <v>754</v>
+      </c>
+      <c r="C505" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="E505" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="506" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A506">
+        <v>74</v>
+      </c>
+      <c r="B506" t="s">
+        <v>761</v>
+      </c>
+      <c r="C506" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E506" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="507" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A507">
+        <v>74</v>
+      </c>
+      <c r="B507" t="s">
+        <v>761</v>
+      </c>
+      <c r="C507" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E507" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="508" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A508">
+        <v>74</v>
+      </c>
+      <c r="B508" t="s">
+        <v>761</v>
+      </c>
+      <c r="C508" s="7" t="s">
+        <v>762</v>
+      </c>
+      <c r="E508" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="509" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A509">
+        <v>74</v>
+      </c>
+      <c r="B509" t="s">
+        <v>761</v>
+      </c>
+      <c r="C509" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="E509" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="510" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A510">
+        <v>74</v>
+      </c>
+      <c r="B510" t="s">
+        <v>761</v>
+      </c>
+      <c r="C510" s="7" t="s">
+        <v>764</v>
+      </c>
+      <c r="E510" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="511" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A511">
+        <v>74</v>
+      </c>
+      <c r="B511" t="s">
+        <v>761</v>
+      </c>
+      <c r="C511" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="E511" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="512" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A512">
+        <v>74</v>
+      </c>
+      <c r="B512" t="s">
+        <v>761</v>
+      </c>
+      <c r="C512" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="E512" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="513" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A513">
+        <v>74</v>
+      </c>
+      <c r="B513" t="s">
+        <v>761</v>
+      </c>
+      <c r="C513" s="7" t="s">
+        <v>767</v>
+      </c>
+      <c r="E513" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="514" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A514">
+        <v>74</v>
+      </c>
+      <c r="B514" t="s">
+        <v>761</v>
+      </c>
+      <c r="C514" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="E514" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="515" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A515">
+        <v>74</v>
+      </c>
+      <c r="B515" t="s">
+        <v>761</v>
+      </c>
+      <c r="C515" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E515" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="516" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A516">
+        <v>74</v>
+      </c>
+      <c r="B516" t="s">
+        <v>761</v>
+      </c>
+      <c r="C516" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E516" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="517" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A517">
+        <v>74</v>
+      </c>
+      <c r="B517" t="s">
+        <v>761</v>
+      </c>
+      <c r="C517" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E517" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="518" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A518">
+        <v>75</v>
+      </c>
+      <c r="B518" t="s">
+        <v>769</v>
+      </c>
+      <c r="C518" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E518" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="519" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A519">
+        <v>75</v>
+      </c>
+      <c r="B519" t="s">
+        <v>769</v>
+      </c>
+      <c r="C519" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E519" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="520" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A520">
+        <v>75</v>
+      </c>
+      <c r="B520" t="s">
+        <v>769</v>
+      </c>
+      <c r="C520" s="7" t="s">
+        <v>770</v>
+      </c>
+      <c r="E520" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="521" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A521">
+        <v>75</v>
+      </c>
+      <c r="B521" t="s">
+        <v>769</v>
+      </c>
+      <c r="C521" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="E521" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="522" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A522">
+        <v>75</v>
+      </c>
+      <c r="B522" t="s">
+        <v>769</v>
+      </c>
+      <c r="C522" s="7" t="s">
+        <v>772</v>
+      </c>
+      <c r="E522" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="523" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A523">
+        <v>75</v>
+      </c>
+      <c r="B523" t="s">
+        <v>769</v>
+      </c>
+      <c r="C523" s="7" t="s">
+        <v>773</v>
+      </c>
+      <c r="E523" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="524" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A524">
+        <v>75</v>
+      </c>
+      <c r="B524" t="s">
+        <v>769</v>
+      </c>
+      <c r="C524" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E524" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="525" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A525">
+        <v>75</v>
+      </c>
+      <c r="B525" t="s">
+        <v>769</v>
+      </c>
+      <c r="C525" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="E525" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="526" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A526">
+        <v>75</v>
+      </c>
+      <c r="B526" t="s">
+        <v>769</v>
+      </c>
+      <c r="C526" s="7" t="s">
+        <v>774</v>
+      </c>
+      <c r="E526" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
82'ye kadar bölüm eklendi - en
</commit_message>
<xml_diff>
--- a/Levels/en/Wordlist.xlsx
+++ b/Levels/en/Wordlist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2005" uniqueCount="822">
   <si>
     <t>id</t>
   </si>
@@ -2344,18 +2344,167 @@
   </si>
   <si>
     <t>CARS</t>
+  </si>
+  <si>
+    <t>E,U,S,R,S</t>
+  </si>
+  <si>
+    <t>SURE</t>
+  </si>
+  <si>
+    <t>USES</t>
+  </si>
+  <si>
+    <t>SUES</t>
+  </si>
+  <si>
+    <t>USERS</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>N,K,E,S,E</t>
+  </si>
+  <si>
+    <t>SEEN</t>
+  </si>
+  <si>
+    <t>KNEE</t>
+  </si>
+  <si>
+    <t>KNEES</t>
+  </si>
+  <si>
+    <t>KEEN</t>
+  </si>
+  <si>
+    <t>I,S,P,T,L</t>
+  </si>
+  <si>
+    <t>SPIT</t>
+  </si>
+  <si>
+    <t>LIT</t>
+  </si>
+  <si>
+    <t>SPLIT</t>
+  </si>
+  <si>
+    <t>LIST</t>
+  </si>
+  <si>
+    <t>SLIP</t>
+  </si>
+  <si>
+    <t>LIP</t>
+  </si>
+  <si>
+    <t>L,L,A,B,E</t>
+  </si>
+  <si>
+    <t>ABLE</t>
+  </si>
+  <si>
+    <t>BELL</t>
+  </si>
+  <si>
+    <t>LABEL</t>
+  </si>
+  <si>
+    <t>LAB</t>
+  </si>
+  <si>
+    <t>BALL</t>
+  </si>
+  <si>
+    <t>O,O,R,P,M</t>
+  </si>
+  <si>
+    <t>PRO</t>
+  </si>
+  <si>
+    <t>MOP</t>
+  </si>
+  <si>
+    <t>POOR</t>
+  </si>
+  <si>
+    <t>PROM</t>
+  </si>
+  <si>
+    <t>PROMO</t>
+  </si>
+  <si>
+    <t>ROOM</t>
+  </si>
+  <si>
+    <t>R,U,B,G,Y</t>
+  </si>
+  <si>
+    <t>BUG</t>
+  </si>
+  <si>
+    <t>GUY</t>
+  </si>
+  <si>
+    <t>BUY</t>
+  </si>
+  <si>
+    <t>RUG</t>
+  </si>
+  <si>
+    <t>RUBY</t>
+  </si>
+  <si>
+    <t>BURY</t>
+  </si>
+  <si>
+    <t>RUGBY</t>
+  </si>
+  <si>
+    <t>E,L,K,S,I</t>
+  </si>
+  <si>
+    <t>SILK</t>
+  </si>
+  <si>
+    <t>LIE</t>
+  </si>
+  <si>
+    <t>ISLE</t>
+  </si>
+  <si>
+    <t>SKI</t>
+  </si>
+  <si>
+    <t>LIKE</t>
+  </si>
+  <si>
+    <t>LIES</t>
+  </si>
+  <si>
+    <t>LIKES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2419,20 +2568,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2713,10 +2863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F526"/>
+  <dimension ref="A1:F578"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
-      <selection activeCell="F360" sqref="F360"/>
+    <sheetView tabSelected="1" topLeftCell="A563" workbookViewId="0">
+      <selection activeCell="E578" sqref="E578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10900,6 +11050,734 @@
         <v>46</v>
       </c>
     </row>
+    <row r="527" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A527">
+        <v>76</v>
+      </c>
+      <c r="B527" t="s">
+        <v>775</v>
+      </c>
+      <c r="C527" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="E527" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="528" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A528">
+        <v>76</v>
+      </c>
+      <c r="B528" t="s">
+        <v>775</v>
+      </c>
+      <c r="C528" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="E528" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="529" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A529">
+        <v>76</v>
+      </c>
+      <c r="B529" t="s">
+        <v>775</v>
+      </c>
+      <c r="C529" s="9" t="s">
+        <v>776</v>
+      </c>
+      <c r="E529" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="530" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A530">
+        <v>76</v>
+      </c>
+      <c r="B530" t="s">
+        <v>775</v>
+      </c>
+      <c r="C530" s="9" t="s">
+        <v>777</v>
+      </c>
+      <c r="E530" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="531" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A531">
+        <v>76</v>
+      </c>
+      <c r="B531" t="s">
+        <v>775</v>
+      </c>
+      <c r="C531" s="9" t="s">
+        <v>778</v>
+      </c>
+      <c r="E531" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="532" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A532">
+        <v>76</v>
+      </c>
+      <c r="B532" t="s">
+        <v>775</v>
+      </c>
+      <c r="C532" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="E532" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="533" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A533">
+        <v>76</v>
+      </c>
+      <c r="B533" t="s">
+        <v>775</v>
+      </c>
+      <c r="C533" s="9" t="s">
+        <v>779</v>
+      </c>
+      <c r="E533" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="534" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A534">
+        <v>76</v>
+      </c>
+      <c r="B534" t="s">
+        <v>775</v>
+      </c>
+      <c r="C534" s="9" t="s">
+        <v>780</v>
+      </c>
+      <c r="E534" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="535" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A535">
+        <v>77</v>
+      </c>
+      <c r="B535" t="s">
+        <v>781</v>
+      </c>
+      <c r="C535" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="E535" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="536" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A536">
+        <v>77</v>
+      </c>
+      <c r="B536" t="s">
+        <v>781</v>
+      </c>
+      <c r="C536" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="E536" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="537" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A537">
+        <v>77</v>
+      </c>
+      <c r="B537" t="s">
+        <v>781</v>
+      </c>
+      <c r="C537" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="E537" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="538" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A538">
+        <v>77</v>
+      </c>
+      <c r="B538" t="s">
+        <v>781</v>
+      </c>
+      <c r="C538" s="9" t="s">
+        <v>784</v>
+      </c>
+      <c r="E538" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="539" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A539">
+        <v>77</v>
+      </c>
+      <c r="B539" t="s">
+        <v>781</v>
+      </c>
+      <c r="C539" s="9" t="s">
+        <v>785</v>
+      </c>
+      <c r="E539" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="540" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A540">
+        <v>77</v>
+      </c>
+      <c r="B540" t="s">
+        <v>781</v>
+      </c>
+      <c r="C540" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="E540" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="541" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A541">
+        <v>78</v>
+      </c>
+      <c r="B541" t="s">
+        <v>786</v>
+      </c>
+      <c r="C541" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="E541" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="542" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A542">
+        <v>78</v>
+      </c>
+      <c r="B542" t="s">
+        <v>786</v>
+      </c>
+      <c r="C542" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="E542" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="543" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A543">
+        <v>78</v>
+      </c>
+      <c r="B543" t="s">
+        <v>786</v>
+      </c>
+      <c r="C543" s="9" t="s">
+        <v>788</v>
+      </c>
+      <c r="E543" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="544" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A544">
+        <v>78</v>
+      </c>
+      <c r="B544" t="s">
+        <v>786</v>
+      </c>
+      <c r="C544" s="9" t="s">
+        <v>789</v>
+      </c>
+      <c r="E544" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="545" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A545">
+        <v>78</v>
+      </c>
+      <c r="B545" t="s">
+        <v>786</v>
+      </c>
+      <c r="C545" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="E545" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="546" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A546">
+        <v>78</v>
+      </c>
+      <c r="B546" t="s">
+        <v>786</v>
+      </c>
+      <c r="C546" s="9" t="s">
+        <v>790</v>
+      </c>
+      <c r="E546" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="547" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A547">
+        <v>78</v>
+      </c>
+      <c r="B547" t="s">
+        <v>786</v>
+      </c>
+      <c r="C547" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="E547" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="548" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A548">
+        <v>78</v>
+      </c>
+      <c r="B548" t="s">
+        <v>786</v>
+      </c>
+      <c r="C548" s="9" t="s">
+        <v>791</v>
+      </c>
+      <c r="E548" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="549" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A549">
+        <v>78</v>
+      </c>
+      <c r="B549" t="s">
+        <v>786</v>
+      </c>
+      <c r="C549" s="9" t="s">
+        <v>792</v>
+      </c>
+      <c r="E549" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="550" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A550">
+        <v>78</v>
+      </c>
+      <c r="B550" t="s">
+        <v>786</v>
+      </c>
+      <c r="C550" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="E550" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="551" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A551">
+        <v>79</v>
+      </c>
+      <c r="B551" t="s">
+        <v>793</v>
+      </c>
+      <c r="C551" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="E551" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="552" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A552">
+        <v>79</v>
+      </c>
+      <c r="B552" t="s">
+        <v>793</v>
+      </c>
+      <c r="C552" s="9" t="s">
+        <v>794</v>
+      </c>
+      <c r="E552" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="553" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A553">
+        <v>79</v>
+      </c>
+      <c r="B553" t="s">
+        <v>793</v>
+      </c>
+      <c r="C553" s="9" t="s">
+        <v>795</v>
+      </c>
+      <c r="E553" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="554" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A554">
+        <v>79</v>
+      </c>
+      <c r="B554" t="s">
+        <v>793</v>
+      </c>
+      <c r="C554" s="9" t="s">
+        <v>796</v>
+      </c>
+      <c r="E554" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="555" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A555">
+        <v>79</v>
+      </c>
+      <c r="B555" t="s">
+        <v>793</v>
+      </c>
+      <c r="C555" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="E555" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="556" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A556">
+        <v>79</v>
+      </c>
+      <c r="B556" t="s">
+        <v>793</v>
+      </c>
+      <c r="C556" s="9" t="s">
+        <v>798</v>
+      </c>
+      <c r="E556" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="557" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A557">
+        <v>79</v>
+      </c>
+      <c r="B557" t="s">
+        <v>793</v>
+      </c>
+      <c r="C557" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="E557" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="558" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A558">
+        <v>80</v>
+      </c>
+      <c r="B558" t="s">
+        <v>799</v>
+      </c>
+      <c r="C558" s="9" t="s">
+        <v>800</v>
+      </c>
+      <c r="E558" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="559" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A559">
+        <v>80</v>
+      </c>
+      <c r="B559" t="s">
+        <v>799</v>
+      </c>
+      <c r="C559" s="9" t="s">
+        <v>801</v>
+      </c>
+      <c r="E559" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="560" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A560">
+        <v>80</v>
+      </c>
+      <c r="B560" t="s">
+        <v>799</v>
+      </c>
+      <c r="C560" s="9" t="s">
+        <v>802</v>
+      </c>
+      <c r="E560" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="561" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A561">
+        <v>80</v>
+      </c>
+      <c r="B561" t="s">
+        <v>799</v>
+      </c>
+      <c r="C561" s="9" t="s">
+        <v>803</v>
+      </c>
+      <c r="E561" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="562" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A562">
+        <v>80</v>
+      </c>
+      <c r="B562" t="s">
+        <v>799</v>
+      </c>
+      <c r="C562" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="E562" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="563" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A563">
+        <v>80</v>
+      </c>
+      <c r="B563" t="s">
+        <v>799</v>
+      </c>
+      <c r="C563" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="E563" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="564" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A564">
+        <v>81</v>
+      </c>
+      <c r="B564" t="s">
+        <v>806</v>
+      </c>
+      <c r="C564" s="9" t="s">
+        <v>807</v>
+      </c>
+      <c r="E564" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="565" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A565">
+        <v>81</v>
+      </c>
+      <c r="B565" t="s">
+        <v>806</v>
+      </c>
+      <c r="C565" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="E565" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="566" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A566">
+        <v>81</v>
+      </c>
+      <c r="B566" t="s">
+        <v>806</v>
+      </c>
+      <c r="C566" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="E566" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="567" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A567">
+        <v>81</v>
+      </c>
+      <c r="B567" t="s">
+        <v>806</v>
+      </c>
+      <c r="C567" s="9" t="s">
+        <v>809</v>
+      </c>
+      <c r="E567" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="568" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A568">
+        <v>81</v>
+      </c>
+      <c r="B568" t="s">
+        <v>806</v>
+      </c>
+      <c r="C568" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="E568" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="569" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A569">
+        <v>81</v>
+      </c>
+      <c r="B569" t="s">
+        <v>806</v>
+      </c>
+      <c r="C569" s="9" t="s">
+        <v>811</v>
+      </c>
+      <c r="E569" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="570" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A570">
+        <v>81</v>
+      </c>
+      <c r="B570" t="s">
+        <v>806</v>
+      </c>
+      <c r="C570" s="9" t="s">
+        <v>812</v>
+      </c>
+      <c r="E570" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="571" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A571">
+        <v>81</v>
+      </c>
+      <c r="B571" t="s">
+        <v>806</v>
+      </c>
+      <c r="C571" s="9" t="s">
+        <v>813</v>
+      </c>
+      <c r="E571" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="572" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A572">
+        <v>82</v>
+      </c>
+      <c r="B572" t="s">
+        <v>814</v>
+      </c>
+      <c r="C572" s="9" t="s">
+        <v>815</v>
+      </c>
+      <c r="E572" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="573" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A573">
+        <v>82</v>
+      </c>
+      <c r="B573" t="s">
+        <v>814</v>
+      </c>
+      <c r="C573" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="E573" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="574" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A574">
+        <v>82</v>
+      </c>
+      <c r="B574" t="s">
+        <v>814</v>
+      </c>
+      <c r="C574" s="9" t="s">
+        <v>817</v>
+      </c>
+      <c r="E574" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="575" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A575">
+        <v>82</v>
+      </c>
+      <c r="B575" t="s">
+        <v>814</v>
+      </c>
+      <c r="C575" s="9" t="s">
+        <v>818</v>
+      </c>
+      <c r="E575" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="576" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A576">
+        <v>82</v>
+      </c>
+      <c r="B576" t="s">
+        <v>814</v>
+      </c>
+      <c r="C576" s="9" t="s">
+        <v>819</v>
+      </c>
+      <c r="E576" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="577" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A577">
+        <v>82</v>
+      </c>
+      <c r="B577" t="s">
+        <v>814</v>
+      </c>
+      <c r="C577" s="9" t="s">
+        <v>820</v>
+      </c>
+      <c r="E577" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="578" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A578">
+        <v>82</v>
+      </c>
+      <c r="B578" t="s">
+        <v>814</v>
+      </c>
+      <c r="C578" s="9" t="s">
+        <v>821</v>
+      </c>
+      <c r="E578" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>